<commit_message>
[#1199980645336559] all test cases finished
</commit_message>
<xml_diff>
--- a/pentaho/test/SP-0.2/test-case-A/inputs/input.xlsx
+++ b/pentaho/test/SP-0.2/test-case-A/inputs/input.xlsx
@@ -8,19 +8,38 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ramon.ecung\Projects\data-warehouse\pentaho\test\SP-0.2\test-case-A\inputs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F75A4832-BBAF-4B0E-90BA-D0CBDEFB12A8}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5444DAC7-ACA9-40A2-A326-352B9CC68036}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="5955" yWindow="7515" windowWidth="13800" windowHeight="9360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="input" sheetId="1" r:id="rId1"/>
+    <sheet name="expected_output" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+  <si>
+    <t>tool_pid</t>
+  </si>
+  <si>
+    <t>tool_code</t>
+  </si>
+  <si>
+    <t>tool_type</t>
+  </si>
+  <si>
+    <t>tool_price</t>
+  </si>
+  <si>
+    <t>tool_inventory_start_date</t>
+  </si>
+  <si>
+    <t>tool_inventory_end_date</t>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -502,9 +521,8 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -860,16 +878,33 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="E2"/>
+  <dimension ref="A1:F1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G1" sqref="A1:G2"/>
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="2" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E2" s="1"/>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>